<commit_message>
update 27 covid shablon
</commit_message>
<xml_diff>
--- a/help/27_COVID_19_svod.xlsx
+++ b/help/27_COVID_19_svod.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharinM\Desktop\Загрузки_временные\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MedovikovOE\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="120">
   <si>
     <t>№ п/п</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>СПб ГБУЗ "Городская больница Святого Великомученика Георгия"</t>
+  </si>
+  <si>
+    <t>ООО "Сиквенс"</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1950,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1965,54 +1993,25 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2024,12 +2023,10 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2051,25 +2048,25 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2080,6 +2077,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2752,13 +2755,13 @@
   <sheetPr codeName="Лист1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG73"/>
+  <dimension ref="A1:AG74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AB54" sqref="AB54"/>
+      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2819,72 +2822,72 @@
       <c r="AB2" s="23"/>
     </row>
     <row r="3" spans="1:28" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="170" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="180" t="s">
+      <c r="A3" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="168" t="s">
+      <c r="C3" s="180" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="172" t="s">
+      <c r="D3" s="183" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="173" t="s">
+      <c r="E3" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="183" t="s">
+      <c r="F3" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="188" t="s">
+      <c r="G3" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="189"/>
-      <c r="I3" s="189"/>
-      <c r="J3" s="189"/>
-      <c r="K3" s="189"/>
-      <c r="L3" s="189"/>
-      <c r="M3" s="189"/>
-      <c r="N3" s="189"/>
-      <c r="O3" s="189"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="177" t="s">
+      <c r="Q3" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="179" t="s">
+      <c r="R3" s="188" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="175" t="s">
+      <c r="S3" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="176"/>
-      <c r="U3" s="185" t="s">
+      <c r="T3" s="173"/>
+      <c r="U3" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="176"/>
-      <c r="W3" s="184" t="s">
+      <c r="V3" s="173"/>
+      <c r="W3" s="172" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="176"/>
-      <c r="Y3" s="187" t="s">
+      <c r="X3" s="173"/>
+      <c r="Y3" s="177" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="176"/>
-      <c r="AA3" s="186" t="s">
+      <c r="Z3" s="173"/>
+      <c r="AA3" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="AB3" s="181" t="s">
+      <c r="AB3" s="168" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="152.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="171"/>
-      <c r="B4" s="169"/>
-      <c r="C4" s="169"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="174"/>
-      <c r="F4" s="178"/>
+      <c r="A4" s="182"/>
+      <c r="B4" s="176"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="171"/>
       <c r="G4" s="26" t="s">
         <v>15</v>
       </c>
@@ -2915,8 +2918,8 @@
       <c r="P4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="178"/>
-      <c r="R4" s="169"/>
+      <c r="Q4" s="171"/>
+      <c r="R4" s="176"/>
       <c r="S4" s="27" t="s">
         <v>25</v>
       </c>
@@ -2941,8 +2944,8 @@
       <c r="Z4" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" s="169"/>
-      <c r="AB4" s="182"/>
+      <c r="AA4" s="176"/>
+      <c r="AB4" s="169"/>
     </row>
     <row r="5" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
@@ -3500,7 +3503,7 @@
         <v>#N/A</v>
       </c>
       <c r="E10" s="83" t="e">
-        <f t="shared" ref="E10:AB10" si="3">SUM(E11:E37)</f>
+        <f t="shared" ref="E10:Z10" si="3">SUM(E11:E37)</f>
         <v>#N/A</v>
       </c>
       <c r="F10" s="83" t="e">
@@ -6635,7 +6638,7 @@
         <v>#N/A</v>
       </c>
       <c r="E38" s="152" t="e">
-        <f t="shared" ref="E38:AB38" si="4">SUM(E39:E52)</f>
+        <f t="shared" ref="E38:Z38" si="4">SUM(E39:E52)</f>
         <v>#N/A</v>
       </c>
       <c r="F38" s="152" t="e">
@@ -8310,7 +8313,7 @@
         <v>#N/A</v>
       </c>
       <c r="E53" s="151" t="e">
-        <f t="shared" ref="E53:AA53" si="5">SUM(E54:E73)</f>
+        <f t="shared" ref="E53:Z53" si="5">SUM(E54:E73)</f>
         <v>#N/A</v>
       </c>
       <c r="F53" s="151" t="e">
@@ -10646,15 +10649,120 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="74" spans="1:28" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="166">
+        <v>64</v>
+      </c>
+      <c r="B74" s="164" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C74" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="D74" s="47" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E74" s="48" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F74" s="49" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P74" s="50" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q74" s="47" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R74" s="47" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S74" s="47" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T74" s="47" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U74" s="51" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V74" s="51" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W74" s="52" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X74" s="52" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y74" s="53" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z74" s="53" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA74" s="51" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AB74" s="54" t="e">
+        <f>VLOOKUP($C74,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="G3:O3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:D4"/>
@@ -10663,6 +10771,13 @@
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="10" fitToHeight="0" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -10695,107 +10810,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="207" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="206" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="193" t="s">
+      <c r="C1" s="208" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="194" t="s">
+      <c r="D1" s="209" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="195" t="s">
+      <c r="E1" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="200" t="s">
+      <c r="F1" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
-      <c r="M1" s="191"/>
-      <c r="N1" s="191"/>
-      <c r="O1" s="191"/>
-      <c r="P1" s="201" t="s">
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="199" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="201" t="s">
+      <c r="Q1" s="199" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="201" t="s">
+      <c r="R1" s="199" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="191"/>
-      <c r="T1" s="203" t="s">
+      <c r="S1" s="198"/>
+      <c r="T1" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="191"/>
-      <c r="V1" s="204" t="s">
+      <c r="U1" s="198"/>
+      <c r="V1" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="191"/>
-      <c r="X1" s="205" t="s">
+      <c r="W1" s="198"/>
+      <c r="X1" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="191"/>
-      <c r="Z1" s="202" t="s">
+      <c r="Y1" s="198"/>
+      <c r="Z1" s="200" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="202" t="s">
+      <c r="AA1" s="200" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="207" t="s">
+      <c r="AB1" s="205" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" s="196" t="s">
+      <c r="AC1" s="194" t="s">
         <v>105</v>
       </c>
       <c r="AD1" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" s="206"/>
-      <c r="AF1" s="197" t="s">
+      <c r="AE1" s="204"/>
+      <c r="AF1" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="198" t="s">
+      <c r="AG1" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="208" t="s">
+      <c r="AH1" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="AI1" s="209" t="s">
+      <c r="AI1" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="209" t="s">
+      <c r="AJ1" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="209" t="s">
+      <c r="AK1" s="192" t="s">
         <v>90</v>
       </c>
-      <c r="AL1" s="199"/>
+      <c r="AL1" s="191"/>
       <c r="AM1" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="210" t="s">
+      <c r="AN1" s="193" t="s">
         <v>11</v>
       </c>
-      <c r="AO1" s="199"/>
+      <c r="AO1" s="191"/>
       <c r="AP1" s="126" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:42" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="191"/>
-      <c r="B2" s="191"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
+      <c r="A2" s="198"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
       <c r="F2" s="100" t="s">
         <v>15</v>
       </c>
@@ -10826,8 +10941,8 @@
       <c r="O2" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="191"/>
-      <c r="Q2" s="191"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
       <c r="R2" s="101" t="s">
         <v>25</v>
       </c>
@@ -10852,19 +10967,19 @@
       <c r="Y2" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="191"/>
-      <c r="AA2" s="191"/>
-      <c r="AB2" s="207"/>
-      <c r="AC2" s="196"/>
+      <c r="Z2" s="198"/>
+      <c r="AA2" s="198"/>
+      <c r="AB2" s="205"/>
+      <c r="AC2" s="194"/>
       <c r="AD2" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="AE2" s="206"/>
-      <c r="AF2" s="197"/>
-      <c r="AG2" s="199"/>
-      <c r="AH2" s="199"/>
-      <c r="AI2" s="199"/>
-      <c r="AJ2" s="199"/>
+      <c r="AE2" s="204"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="191"/>
+      <c r="AH2" s="191"/>
+      <c r="AI2" s="191"/>
+      <c r="AJ2" s="191"/>
       <c r="AK2" s="118" t="s">
         <v>25</v>
       </c>
@@ -10998,7 +11113,7 @@
         <f>W3-Y3</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="206"/>
+      <c r="AE3" s="204"/>
       <c r="AF3" s="127">
         <f>IF(C3&gt;=U3,0,1)</f>
         <v>0</v>
@@ -18801,11 +18916,11 @@
   </sheetData>
   <autoFilter ref="A3:AB43"/>
   <mergeCells count="24">
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
@@ -18820,11 +18935,11 @@
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AE1:AE3"/>
     <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
@@ -19820,68 +19935,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="207" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="212" t="s">
+      <c r="B1" s="217" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="213" t="s">
+      <c r="C1" s="218" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="194" t="s">
+      <c r="D1" s="209" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="195" t="s">
+      <c r="E1" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="195" t="s">
+      <c r="F1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="211"/>
-      <c r="H1" s="211"/>
-      <c r="I1" s="211"/>
-      <c r="J1" s="211"/>
-      <c r="K1" s="211"/>
-      <c r="L1" s="211"/>
-      <c r="M1" s="211"/>
-      <c r="N1" s="211"/>
-      <c r="O1" s="211"/>
-      <c r="P1" s="215" t="s">
+      <c r="G1" s="212"/>
+      <c r="H1" s="212"/>
+      <c r="I1" s="212"/>
+      <c r="J1" s="212"/>
+      <c r="K1" s="212"/>
+      <c r="L1" s="212"/>
+      <c r="M1" s="212"/>
+      <c r="N1" s="212"/>
+      <c r="O1" s="212"/>
+      <c r="P1" s="213" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="215" t="s">
+      <c r="Q1" s="213" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="215" t="s">
+      <c r="R1" s="213" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="211"/>
-      <c r="T1" s="216" t="s">
+      <c r="S1" s="212"/>
+      <c r="T1" s="214" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="211"/>
-      <c r="V1" s="217" t="s">
+      <c r="U1" s="212"/>
+      <c r="V1" s="215" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="211"/>
-      <c r="X1" s="218" t="s">
+      <c r="W1" s="212"/>
+      <c r="X1" s="216" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="211"/>
-      <c r="Z1" s="214" t="s">
+      <c r="Y1" s="212"/>
+      <c r="Z1" s="211" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="214" t="s">
+      <c r="AA1" s="211" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="220.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="211"/>
-      <c r="B2" s="211"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
+      <c r="A2" s="212"/>
+      <c r="B2" s="212"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
       <c r="F2" s="130" t="s">
         <v>15</v>
       </c>
@@ -19912,8 +20027,8 @@
       <c r="O2" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="211"/>
-      <c r="Q2" s="211"/>
+      <c r="P2" s="212"/>
+      <c r="Q2" s="212"/>
       <c r="R2" s="131" t="s">
         <v>25</v>
       </c>
@@ -19938,8 +20053,8 @@
       <c r="Y2" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="211"/>
-      <c r="AA2" s="211"/>
+      <c r="Z2" s="212"/>
+      <c r="AA2" s="212"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="134" t="s">
@@ -22862,6 +22977,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:O1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="P1:P2"/>
@@ -22870,12 +22991,6 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="F1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E100">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
update mo by ogrn
</commit_message>
<xml_diff>
--- a/help/27_COVID_19_svod.xlsx
+++ b/help/27_COVID_19_svod.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="120">
   <si>
     <t>№ п/п</t>
   </si>
@@ -1530,7 +1530,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1966,35 +1966,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2009,25 +1988,54 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2039,10 +2047,12 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2064,25 +2074,25 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2093,15 +2103,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2119,7 +2120,7 @@
     <cellStyle name="Обычный 6" xfId="8"/>
     <cellStyle name="Обычный 7" xfId="10"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="79">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2177,6 +2178,356 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2774,13 +3125,13 @@
   <sheetPr codeName="Лист1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AG74"/>
+  <dimension ref="A1:AG95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomRight" activeCell="A79" sqref="A79:D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2841,72 +3192,72 @@
       <c r="AB2" s="23"/>
     </row>
     <row r="3" spans="1:28" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="182" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="190" t="s">
+      <c r="A3" s="173" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="183" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="181" t="s">
+      <c r="C3" s="171" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="184" t="s">
+      <c r="D3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="185" t="s">
+      <c r="E3" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="179" t="s">
+      <c r="G3" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="180"/>
-      <c r="L3" s="180"/>
-      <c r="M3" s="180"/>
-      <c r="N3" s="180"/>
-      <c r="O3" s="180"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="192"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="188" t="s">
+      <c r="Q3" s="180" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="189" t="s">
+      <c r="R3" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="187" t="s">
+      <c r="S3" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="174"/>
-      <c r="U3" s="175" t="s">
+      <c r="T3" s="179"/>
+      <c r="U3" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="174"/>
-      <c r="W3" s="173" t="s">
+      <c r="V3" s="179"/>
+      <c r="W3" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="174"/>
-      <c r="Y3" s="178" t="s">
+      <c r="X3" s="179"/>
+      <c r="Y3" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="174"/>
-      <c r="AA3" s="176" t="s">
+      <c r="Z3" s="179"/>
+      <c r="AA3" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="AB3" s="169" t="s">
+      <c r="AB3" s="184" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="152.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="183"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="172"/>
+      <c r="A4" s="174"/>
+      <c r="B4" s="172"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="181"/>
       <c r="G4" s="26" t="s">
         <v>15</v>
       </c>
@@ -2937,8 +3288,8 @@
       <c r="P4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="172"/>
-      <c r="R4" s="177"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="172"/>
       <c r="S4" s="27" t="s">
         <v>25</v>
       </c>
@@ -2963,8 +3314,8 @@
       <c r="Z4" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" s="177"/>
-      <c r="AB4" s="170"/>
+      <c r="AA4" s="172"/>
+      <c r="AB4" s="185"/>
     </row>
     <row r="5" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
@@ -4854,112 +5205,112 @@
       <c r="A22" s="79">
         <v>14</v>
       </c>
-      <c r="B22" s="70" t="e">
+      <c r="B22" s="70">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>189004</v>
       </c>
       <c r="C22" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="85" t="e">
+      <c r="D22" s="85">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E22" s="14" t="e">
+        <v>350</v>
+      </c>
+      <c r="E22" s="14">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="15" t="e">
+        <v>64256</v>
+      </c>
+      <c r="F22" s="15">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P22" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P22" s="10">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q22" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="12">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R22" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="R22" s="12">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S22" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S22" s="12">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T22" s="12" t="e">
+        <v>64286</v>
+      </c>
+      <c r="T22" s="12">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U22" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U22" s="9">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V22" s="9" t="e">
+        <v>68506</v>
+      </c>
+      <c r="V22" s="9">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W22" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W22" s="11">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X22" s="11" t="e">
+        <v>10462</v>
+      </c>
+      <c r="X22" s="11">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y22" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="13">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z22" s="13" t="e">
+        <v>10364</v>
+      </c>
+      <c r="Z22" s="13">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA22" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="9">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB22" s="46" t="e">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="46">
         <f>VLOOKUP($C22,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5639,112 +5990,112 @@
       <c r="A29" s="79">
         <v>21</v>
       </c>
-      <c r="B29" s="70" t="e">
+      <c r="B29" s="70">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>186700</v>
       </c>
       <c r="C29" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="85" t="e">
+      <c r="D29" s="85">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E29" s="14" t="e">
+        <v>120</v>
+      </c>
+      <c r="E29" s="14">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F29" s="15" t="e">
+        <v>37435</v>
+      </c>
+      <c r="F29" s="15">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P29" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P29" s="10">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q29" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="12">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R29" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="R29" s="12">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S29" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S29" s="12">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T29" s="12" t="e">
+        <v>36538</v>
+      </c>
+      <c r="T29" s="12">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U29" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U29" s="9">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V29" s="9" t="e">
+        <v>37127</v>
+      </c>
+      <c r="V29" s="9">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W29" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W29" s="11">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X29" s="11" t="e">
+        <v>1860</v>
+      </c>
+      <c r="X29" s="11">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y29" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="13">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z29" s="13" t="e">
+        <v>1852</v>
+      </c>
+      <c r="Z29" s="13">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA29" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="9">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB29" s="46" t="e">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="46">
         <f>VLOOKUP($C29,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC29" s="7"/>
     </row>
@@ -6090,112 +6441,112 @@
       <c r="A33" s="79">
         <v>25</v>
       </c>
-      <c r="B33" s="70" t="e">
+      <c r="B33" s="70">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>182884</v>
       </c>
       <c r="C33" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="85" t="e">
+      <c r="D33" s="85">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E33" s="14" t="e">
+        <v>100</v>
+      </c>
+      <c r="E33" s="14">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F33" s="15" t="e">
+        <v>4470</v>
+      </c>
+      <c r="F33" s="15">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P33" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P33" s="10">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q33" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="12">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R33" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="R33" s="12">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S33" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S33" s="12">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T33" s="12" t="e">
+        <v>4470</v>
+      </c>
+      <c r="T33" s="12">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U33" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U33" s="9">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V33" s="9" t="e">
+        <v>4685</v>
+      </c>
+      <c r="V33" s="9">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W33" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W33" s="11">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X33" s="11" t="e">
+        <v>962</v>
+      </c>
+      <c r="X33" s="11">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y33" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="13">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z33" s="13" t="e">
+        <v>930</v>
+      </c>
+      <c r="Z33" s="13">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA33" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="9">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB33" s="46" t="e">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="46">
         <f>VLOOKUP($C33,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6869,224 +7220,224 @@
       <c r="A40" s="150">
         <v>31</v>
       </c>
-      <c r="B40" s="79" t="e">
+      <c r="B40" s="79">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>800109</v>
       </c>
       <c r="C40" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="12" t="e">
+      <c r="D40" s="12">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E40" s="14" t="e">
+        <v>300</v>
+      </c>
+      <c r="E40" s="14">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F40" s="15" t="e">
+        <v>35684</v>
+      </c>
+      <c r="F40" s="15">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P40" s="10">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q40" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="12">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R40" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="R40" s="12">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S40" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S40" s="12">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T40" s="12" t="e">
+        <v>19014</v>
+      </c>
+      <c r="T40" s="12">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U40" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U40" s="9">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V40" s="9" t="e">
+        <v>35667</v>
+      </c>
+      <c r="V40" s="9">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W40" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W40" s="11">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X40" s="11" t="e">
+        <v>2872</v>
+      </c>
+      <c r="X40" s="11">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y40" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="13">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z40" s="13" t="e">
+        <v>2656</v>
+      </c>
+      <c r="Z40" s="13">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA40" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="9">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB40" s="46" t="e">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="46">
         <f>VLOOKUP($C40,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:28" ht="69.75" x14ac:dyDescent="0.25">
       <c r="A41" s="149">
         <v>32</v>
       </c>
-      <c r="B41" s="79" t="e">
+      <c r="B41" s="79">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>731171</v>
       </c>
       <c r="C41" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="D41" s="12" t="e">
+      <c r="D41" s="12">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E41" s="14" t="e">
+        <v>400</v>
+      </c>
+      <c r="E41" s="14">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F41" s="15" t="e">
+        <v>3217</v>
+      </c>
+      <c r="F41" s="15">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P41" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P41" s="10">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q41" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="12">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R41" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="R41" s="12">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S41" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S41" s="12">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T41" s="12" t="e">
+        <v>2916</v>
+      </c>
+      <c r="T41" s="12">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U41" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U41" s="9">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V41" s="9" t="e">
+        <v>3320</v>
+      </c>
+      <c r="V41" s="9">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W41" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W41" s="11">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X41" s="11" t="e">
+        <v>240</v>
+      </c>
+      <c r="X41" s="11">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y41" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="13">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z41" s="13" t="e">
+        <v>159</v>
+      </c>
+      <c r="Z41" s="13">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA41" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="9">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB41" s="46" t="e">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="46">
         <f>VLOOKUP($C41,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="59.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7877,112 +8228,112 @@
       <c r="A49" s="149">
         <v>40</v>
       </c>
-      <c r="B49" s="79" t="e">
+      <c r="B49" s="79">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>731178</v>
       </c>
       <c r="C49" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="12" t="e">
+      <c r="D49" s="12">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E49" s="14" t="e">
+        <v>300</v>
+      </c>
+      <c r="E49" s="14">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F49" s="15" t="e">
+        <v>52813</v>
+      </c>
+      <c r="F49" s="15">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P49" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P49" s="10">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q49" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="12">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R49" s="12" t="e">
+        <v>59</v>
+      </c>
+      <c r="R49" s="12">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S49" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S49" s="12">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T49" s="12" t="e">
+        <v>26188</v>
+      </c>
+      <c r="T49" s="12">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U49" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U49" s="9">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V49" s="9" t="e">
+        <v>52481</v>
+      </c>
+      <c r="V49" s="9">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W49" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W49" s="11">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X49" s="11" t="e">
+        <v>728</v>
+      </c>
+      <c r="X49" s="11">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y49" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="13">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z49" s="13" t="e">
+        <v>720</v>
+      </c>
+      <c r="Z49" s="13">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA49" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="9">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB49" s="46" t="e">
+        <v>20</v>
+      </c>
+      <c r="AB49" s="46">
         <f>VLOOKUP($C49,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:28" s="97" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9660,7 +10011,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="166">
         <v>55</v>
       </c>
@@ -9772,7 +10123,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="166">
         <v>56</v>
       </c>
@@ -9884,7 +10235,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="166">
         <v>57</v>
       </c>
@@ -9996,7 +10347,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="166">
         <v>58</v>
       </c>
@@ -10108,119 +10459,119 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="166">
         <v>59</v>
       </c>
-      <c r="B69" s="163" t="e">
+      <c r="B69" s="163">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,2,0)</f>
-        <v>#N/A</v>
+        <v>78780154</v>
       </c>
       <c r="C69" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="D69" s="12" t="e">
+      <c r="D69" s="12">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E69" s="14" t="e">
+        <v>200</v>
+      </c>
+      <c r="E69" s="14">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F69" s="15" t="e">
+        <v>5877</v>
+      </c>
+      <c r="F69" s="15">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="G69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="I69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="K69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="L69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="M69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="N69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="O69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P69" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="P69" s="10">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q69" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="12">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R69" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="R69" s="12">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S69" s="12" t="e">
+        <v>0</v>
+      </c>
+      <c r="S69" s="12">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T69" s="12" t="e">
+        <v>5877</v>
+      </c>
+      <c r="T69" s="12">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U69" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="U69" s="9">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V69" s="9" t="e">
+        <v>5877</v>
+      </c>
+      <c r="V69" s="9">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W69" s="11" t="e">
+        <v>0</v>
+      </c>
+      <c r="W69" s="11">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X69" s="11" t="e">
+        <v>1582</v>
+      </c>
+      <c r="X69" s="11">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y69" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="13">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z69" s="13" t="e">
+        <v>1582</v>
+      </c>
+      <c r="Z69" s="13">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA69" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AA69" s="9">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB69" s="46" t="e">
+        <v>0</v>
+      </c>
+      <c r="AB69" s="46">
         <f>VLOOKUP($C69,'Для заполнения'!$A$3:$AA$100,COLUMN()-1,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="70" spans="1:28" s="97" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:33" s="97" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="166">
         <v>60</v>
       </c>
@@ -10332,7 +10683,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="166">
         <v>61</v>
       </c>
@@ -10444,7 +10795,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="8" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" s="8" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="166">
         <v>62</v>
       </c>
@@ -10556,7 +10907,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="97" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" s="97" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="166">
         <v>63</v>
       </c>
@@ -10668,8 +11019,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="8" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="220">
+    <row r="74" spans="1:33" s="8" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="170">
         <v>64</v>
       </c>
       <c r="B74" s="164" t="e">
@@ -10780,8 +11131,117 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="79" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD79"/>
+      <c r="AE79"/>
+      <c r="AF79"/>
+      <c r="AG79"/>
+    </row>
+    <row r="80" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD80"/>
+      <c r="AE80"/>
+      <c r="AF80"/>
+      <c r="AG80"/>
+    </row>
+    <row r="81" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD81"/>
+      <c r="AE81"/>
+      <c r="AF81"/>
+      <c r="AG81"/>
+    </row>
+    <row r="82" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD82"/>
+      <c r="AE82"/>
+      <c r="AF82"/>
+      <c r="AG82"/>
+    </row>
+    <row r="83" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD83"/>
+      <c r="AE83"/>
+      <c r="AF83"/>
+      <c r="AG83"/>
+    </row>
+    <row r="84" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD84"/>
+      <c r="AE84"/>
+      <c r="AF84"/>
+      <c r="AG84"/>
+    </row>
+    <row r="85" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD85"/>
+      <c r="AE85"/>
+      <c r="AF85"/>
+      <c r="AG85"/>
+    </row>
+    <row r="86" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD86"/>
+      <c r="AE86"/>
+      <c r="AF86"/>
+      <c r="AG86"/>
+    </row>
+    <row r="87" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD87"/>
+      <c r="AE87"/>
+      <c r="AF87"/>
+      <c r="AG87"/>
+    </row>
+    <row r="88" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD88"/>
+      <c r="AE88"/>
+      <c r="AF88"/>
+      <c r="AG88"/>
+    </row>
+    <row r="89" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD89"/>
+      <c r="AE89"/>
+      <c r="AF89"/>
+      <c r="AG89"/>
+    </row>
+    <row r="90" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD90"/>
+      <c r="AE90"/>
+      <c r="AF90"/>
+      <c r="AG90"/>
+    </row>
+    <row r="91" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD91"/>
+      <c r="AE91"/>
+      <c r="AF91"/>
+      <c r="AG91"/>
+    </row>
+    <row r="92" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD92"/>
+      <c r="AE92"/>
+      <c r="AF92"/>
+      <c r="AG92"/>
+    </row>
+    <row r="93" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD93"/>
+      <c r="AE93"/>
+      <c r="AF93"/>
+      <c r="AG93"/>
+    </row>
+    <row r="94" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD94"/>
+      <c r="AE94"/>
+      <c r="AF94"/>
+      <c r="AG94"/>
+    </row>
+    <row r="95" spans="30:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD95"/>
+      <c r="AE95"/>
+      <c r="AF95"/>
+      <c r="AG95"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="G3:O3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:D4"/>
@@ -10790,13 +11250,6 @@
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="10" fitToHeight="0" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -10809,9 +11262,9 @@
   <dimension ref="A1:AP100"/>
   <sheetViews>
     <sheetView zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100:AA100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -10829,107 +11282,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="207" t="s">
+      <c r="B1" s="193" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="209" t="s">
+      <c r="C1" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="210" t="s">
+      <c r="D1" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="211" t="s">
+      <c r="E1" s="198" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="198" t="s">
+      <c r="F1" s="203" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="199"/>
-      <c r="K1" s="199"/>
-      <c r="L1" s="199"/>
-      <c r="M1" s="199"/>
-      <c r="N1" s="199"/>
-      <c r="O1" s="199"/>
-      <c r="P1" s="200" t="s">
+      <c r="G1" s="194"/>
+      <c r="H1" s="194"/>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
+      <c r="L1" s="194"/>
+      <c r="M1" s="194"/>
+      <c r="N1" s="194"/>
+      <c r="O1" s="194"/>
+      <c r="P1" s="204" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="200" t="s">
+      <c r="Q1" s="204" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="200" t="s">
+      <c r="R1" s="204" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="199"/>
-      <c r="T1" s="202" t="s">
+      <c r="S1" s="194"/>
+      <c r="T1" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="199"/>
-      <c r="V1" s="203" t="s">
+      <c r="U1" s="194"/>
+      <c r="V1" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="199"/>
-      <c r="X1" s="204" t="s">
+      <c r="W1" s="194"/>
+      <c r="X1" s="208" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="199"/>
-      <c r="Z1" s="201" t="s">
+      <c r="Y1" s="194"/>
+      <c r="Z1" s="205" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="201" t="s">
+      <c r="AA1" s="205" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="206" t="s">
+      <c r="AB1" s="210" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" s="195" t="s">
+      <c r="AC1" s="199" t="s">
         <v>105</v>
       </c>
       <c r="AD1" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" s="205"/>
-      <c r="AF1" s="196" t="s">
+      <c r="AE1" s="209"/>
+      <c r="AF1" s="200" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="197" t="s">
+      <c r="AG1" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="191" t="s">
+      <c r="AH1" s="211" t="s">
         <v>5</v>
       </c>
-      <c r="AI1" s="193" t="s">
+      <c r="AI1" s="212" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="193" t="s">
+      <c r="AJ1" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="193" t="s">
+      <c r="AK1" s="212" t="s">
         <v>90</v>
       </c>
-      <c r="AL1" s="192"/>
+      <c r="AL1" s="202"/>
       <c r="AM1" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="194" t="s">
+      <c r="AN1" s="213" t="s">
         <v>11</v>
       </c>
-      <c r="AO1" s="192"/>
+      <c r="AO1" s="202"/>
       <c r="AP1" s="126" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:42" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="199"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="209"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
+      <c r="A2" s="194"/>
+      <c r="B2" s="194"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="194"/>
       <c r="F2" s="100" t="s">
         <v>15</v>
       </c>
@@ -10960,8 +11413,8 @@
       <c r="O2" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="199"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194"/>
       <c r="R2" s="101" t="s">
         <v>25</v>
       </c>
@@ -10986,19 +11439,19 @@
       <c r="Y2" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="199"/>
-      <c r="AA2" s="199"/>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="195"/>
+      <c r="Z2" s="194"/>
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="210"/>
+      <c r="AC2" s="199"/>
       <c r="AD2" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="AE2" s="205"/>
-      <c r="AF2" s="196"/>
-      <c r="AG2" s="192"/>
-      <c r="AH2" s="192"/>
-      <c r="AI2" s="192"/>
-      <c r="AJ2" s="192"/>
+      <c r="AE2" s="209"/>
+      <c r="AF2" s="200"/>
+      <c r="AG2" s="202"/>
+      <c r="AH2" s="202"/>
+      <c r="AI2" s="202"/>
+      <c r="AJ2" s="202"/>
       <c r="AK2" s="118" t="s">
         <v>25</v>
       </c>
@@ -11025,11 +11478,11 @@
       <c r="B3" s="154"/>
       <c r="C3" s="105">
         <f t="shared" ref="C3:AA3" si="0">SUM(C4:C100)</f>
-        <v>0</v>
+        <v>1770</v>
       </c>
       <c r="D3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>203752</v>
       </c>
       <c r="E3" s="105">
         <f t="shared" si="0"/>
@@ -11077,7 +11530,7 @@
       </c>
       <c r="P3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="105">
         <f t="shared" si="0"/>
@@ -11085,7 +11538,7 @@
       </c>
       <c r="R3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>159289</v>
       </c>
       <c r="S3" s="105">
         <f t="shared" si="0"/>
@@ -11093,7 +11546,7 @@
       </c>
       <c r="T3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>207663</v>
       </c>
       <c r="U3" s="105">
         <f t="shared" si="0"/>
@@ -11101,7 +11554,7 @@
       </c>
       <c r="V3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18706</v>
       </c>
       <c r="W3" s="105">
         <f t="shared" si="0"/>
@@ -11109,7 +11562,7 @@
       </c>
       <c r="X3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18263</v>
       </c>
       <c r="Y3" s="105">
         <f t="shared" si="0"/>
@@ -11117,11 +11570,11 @@
       </c>
       <c r="Z3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA3" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3" s="160"/>
       <c r="AC3" s="156">
@@ -11132,14 +11585,14 @@
         <f>W3-Y3</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="205"/>
+      <c r="AE3" s="209"/>
       <c r="AF3" s="127">
         <f>IF(C3&gt;=U3,0,1)</f>
         <v>0</v>
       </c>
       <c r="AG3" s="127">
         <f>D3-Пред.отч!D3</f>
-        <v>0</v>
+        <v>203752</v>
       </c>
       <c r="AH3" s="127">
         <f>E3-SUM(F3:O3)</f>
@@ -11149,7 +11602,7 @@
       <c r="AJ3" s="127"/>
       <c r="AK3" s="127">
         <f>R3-S3-Пред.отч!R3</f>
-        <v>0</v>
+        <v>159289</v>
       </c>
       <c r="AL3" s="127">
         <f>IF(S3&lt;=U3,0,1)</f>
@@ -11157,11 +11610,11 @@
       </c>
       <c r="AM3" s="127">
         <f>T3-U3-Пред.отч!T3</f>
-        <v>0</v>
+        <v>207663</v>
       </c>
       <c r="AN3" s="127">
         <f>V3-W3-Пред.отч!V3</f>
-        <v>0</v>
+        <v>18706</v>
       </c>
       <c r="AO3" s="127">
         <f>IF(W3&gt;=Y3,0,1)</f>
@@ -11169,7 +11622,7 @@
       </c>
       <c r="AP3" s="127">
         <f>X3-Y3-Пред.отч!X3</f>
-        <v>0</v>
+        <v>18263</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18372,37 +18825,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A94" s="16"/>
-      <c r="B94" s="154"/>
-      <c r="C94" s="154"/>
-      <c r="D94" s="154"/>
-      <c r="E94" s="154"/>
-      <c r="F94" s="154"/>
-      <c r="G94" s="154"/>
-      <c r="H94" s="154"/>
-      <c r="I94" s="154"/>
-      <c r="J94" s="154"/>
-      <c r="K94" s="154"/>
-      <c r="L94" s="154"/>
-      <c r="M94" s="154"/>
-      <c r="N94" s="154"/>
-      <c r="O94" s="154"/>
-      <c r="P94" s="154"/>
-      <c r="Q94" s="154"/>
-      <c r="R94" s="154"/>
-      <c r="S94" s="154"/>
-      <c r="T94" s="154"/>
-      <c r="U94" s="154"/>
-      <c r="V94" s="154"/>
-      <c r="W94" s="154"/>
-      <c r="X94" s="154"/>
-      <c r="Y94" s="154"/>
-      <c r="Z94" s="154"/>
-      <c r="AA94" s="154"/>
-      <c r="AB94" s="160">
+    <row r="94" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" s="169">
+        <v>189004</v>
+      </c>
+      <c r="C94" s="169">
+        <v>350</v>
+      </c>
+      <c r="D94" s="169">
+        <v>64256</v>
+      </c>
+      <c r="E94" s="169">
+        <v>0</v>
+      </c>
+      <c r="F94" s="169">
+        <v>0</v>
+      </c>
+      <c r="G94" s="169">
+        <v>0</v>
+      </c>
+      <c r="H94" s="169">
+        <v>0</v>
+      </c>
+      <c r="I94" s="169">
+        <v>0</v>
+      </c>
+      <c r="J94" s="169">
+        <v>0</v>
+      </c>
+      <c r="K94" s="169">
+        <v>0</v>
+      </c>
+      <c r="L94" s="169">
+        <v>0</v>
+      </c>
+      <c r="M94" s="169">
+        <v>0</v>
+      </c>
+      <c r="N94" s="169">
+        <v>0</v>
+      </c>
+      <c r="O94" s="169">
+        <v>0</v>
+      </c>
+      <c r="P94" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="169">
+        <v>0</v>
+      </c>
+      <c r="R94" s="169">
+        <v>64286</v>
+      </c>
+      <c r="S94" s="169">
+        <v>0</v>
+      </c>
+      <c r="T94" s="169">
+        <v>68506</v>
+      </c>
+      <c r="U94" s="169">
+        <v>0</v>
+      </c>
+      <c r="V94" s="169">
+        <v>10462</v>
+      </c>
+      <c r="W94" s="169">
+        <v>0</v>
+      </c>
+      <c r="X94" s="169">
+        <v>10364</v>
+      </c>
+      <c r="Y94" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z94" s="169">
+        <v>0</v>
+      </c>
+      <c r="AA94" s="169">
+        <v>0</v>
+      </c>
+      <c r="AB94" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>СПб ГБУЗ "Городская Мариинская больница"</v>
       </c>
       <c r="AC94" s="156">
         <f t="shared" si="9"/>
@@ -18452,37 +18959,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A95" s="16"/>
-      <c r="B95" s="154"/>
-      <c r="C95" s="154"/>
-      <c r="D95" s="154"/>
-      <c r="E95" s="154"/>
-      <c r="F95" s="154"/>
-      <c r="G95" s="154"/>
-      <c r="H95" s="154"/>
-      <c r="I95" s="154"/>
-      <c r="J95" s="154"/>
-      <c r="K95" s="154"/>
-      <c r="L95" s="154"/>
-      <c r="M95" s="154"/>
-      <c r="N95" s="154"/>
-      <c r="O95" s="154"/>
-      <c r="P95" s="154"/>
-      <c r="Q95" s="154"/>
-      <c r="R95" s="154"/>
-      <c r="S95" s="154"/>
-      <c r="T95" s="154"/>
-      <c r="U95" s="154"/>
-      <c r="V95" s="154"/>
-      <c r="W95" s="154"/>
-      <c r="X95" s="154"/>
-      <c r="Y95" s="154"/>
-      <c r="Z95" s="154"/>
-      <c r="AA95" s="154"/>
-      <c r="AB95" s="160">
+    <row r="95" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95" s="169">
+        <v>186700</v>
+      </c>
+      <c r="C95" s="169">
+        <v>120</v>
+      </c>
+      <c r="D95" s="169">
+        <v>37435</v>
+      </c>
+      <c r="E95" s="169">
+        <v>0</v>
+      </c>
+      <c r="F95" s="169">
+        <v>0</v>
+      </c>
+      <c r="G95" s="169">
+        <v>0</v>
+      </c>
+      <c r="H95" s="169">
+        <v>0</v>
+      </c>
+      <c r="I95" s="169">
+        <v>0</v>
+      </c>
+      <c r="J95" s="169">
+        <v>0</v>
+      </c>
+      <c r="K95" s="169">
+        <v>0</v>
+      </c>
+      <c r="L95" s="169">
+        <v>0</v>
+      </c>
+      <c r="M95" s="169">
+        <v>0</v>
+      </c>
+      <c r="N95" s="169">
+        <v>0</v>
+      </c>
+      <c r="O95" s="169">
+        <v>0</v>
+      </c>
+      <c r="P95" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="169">
+        <v>0</v>
+      </c>
+      <c r="R95" s="169">
+        <v>36538</v>
+      </c>
+      <c r="S95" s="169">
+        <v>0</v>
+      </c>
+      <c r="T95" s="169">
+        <v>37127</v>
+      </c>
+      <c r="U95" s="169">
+        <v>0</v>
+      </c>
+      <c r="V95" s="169">
+        <v>1860</v>
+      </c>
+      <c r="W95" s="169">
+        <v>0</v>
+      </c>
+      <c r="X95" s="169">
+        <v>1852</v>
+      </c>
+      <c r="Y95" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z95" s="169">
+        <v>0</v>
+      </c>
+      <c r="AA95" s="169">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>СПб ГБУЗ "Городской клинический онкологический диспансер"</v>
       </c>
       <c r="AC95" s="156">
         <f t="shared" si="9"/>
@@ -18532,37 +19093,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A96" s="16"/>
-      <c r="B96" s="154"/>
-      <c r="C96" s="154"/>
-      <c r="D96" s="154"/>
-      <c r="E96" s="154"/>
-      <c r="F96" s="154"/>
-      <c r="G96" s="154"/>
-      <c r="H96" s="154"/>
-      <c r="I96" s="154"/>
-      <c r="J96" s="154"/>
-      <c r="K96" s="154"/>
-      <c r="L96" s="154"/>
-      <c r="M96" s="154"/>
-      <c r="N96" s="154"/>
-      <c r="O96" s="154"/>
-      <c r="P96" s="154"/>
-      <c r="Q96" s="154"/>
-      <c r="R96" s="154"/>
-      <c r="S96" s="154"/>
-      <c r="T96" s="154"/>
-      <c r="U96" s="154"/>
-      <c r="V96" s="154"/>
-      <c r="W96" s="154"/>
-      <c r="X96" s="154"/>
-      <c r="Y96" s="154"/>
-      <c r="Z96" s="154"/>
-      <c r="AA96" s="154"/>
-      <c r="AB96" s="160">
+    <row r="96" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B96" s="169">
+        <v>182884</v>
+      </c>
+      <c r="C96" s="169">
+        <v>100</v>
+      </c>
+      <c r="D96" s="169">
+        <v>4470</v>
+      </c>
+      <c r="E96" s="169">
+        <v>0</v>
+      </c>
+      <c r="F96" s="169">
+        <v>0</v>
+      </c>
+      <c r="G96" s="169">
+        <v>0</v>
+      </c>
+      <c r="H96" s="169">
+        <v>0</v>
+      </c>
+      <c r="I96" s="169">
+        <v>0</v>
+      </c>
+      <c r="J96" s="169">
+        <v>0</v>
+      </c>
+      <c r="K96" s="169">
+        <v>0</v>
+      </c>
+      <c r="L96" s="169">
+        <v>0</v>
+      </c>
+      <c r="M96" s="169">
+        <v>0</v>
+      </c>
+      <c r="N96" s="169">
+        <v>0</v>
+      </c>
+      <c r="O96" s="169">
+        <v>0</v>
+      </c>
+      <c r="P96" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="169">
+        <v>0</v>
+      </c>
+      <c r="R96" s="169">
+        <v>4470</v>
+      </c>
+      <c r="S96" s="169">
+        <v>0</v>
+      </c>
+      <c r="T96" s="169">
+        <v>4685</v>
+      </c>
+      <c r="U96" s="169">
+        <v>0</v>
+      </c>
+      <c r="V96" s="169">
+        <v>962</v>
+      </c>
+      <c r="W96" s="169">
+        <v>0</v>
+      </c>
+      <c r="X96" s="169">
+        <v>930</v>
+      </c>
+      <c r="Y96" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z96" s="169">
+        <v>0</v>
+      </c>
+      <c r="AA96" s="169">
+        <v>0</v>
+      </c>
+      <c r="AB96" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>СПб ГБУЗ "Городская больница Святой преподобномученицы Елизаветы"</v>
       </c>
       <c r="AC96" s="156">
         <f t="shared" si="9"/>
@@ -18612,37 +19227,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A97" s="16"/>
-      <c r="B97" s="154"/>
-      <c r="C97" s="154"/>
-      <c r="D97" s="154"/>
-      <c r="E97" s="154"/>
-      <c r="F97" s="154"/>
-      <c r="G97" s="154"/>
-      <c r="H97" s="154"/>
-      <c r="I97" s="154"/>
-      <c r="J97" s="154"/>
-      <c r="K97" s="154"/>
-      <c r="L97" s="154"/>
-      <c r="M97" s="154"/>
-      <c r="N97" s="154"/>
-      <c r="O97" s="154"/>
-      <c r="P97" s="154"/>
-      <c r="Q97" s="154"/>
-      <c r="R97" s="154"/>
-      <c r="S97" s="154"/>
-      <c r="T97" s="154"/>
-      <c r="U97" s="154"/>
-      <c r="V97" s="154"/>
-      <c r="W97" s="154"/>
-      <c r="X97" s="154"/>
-      <c r="Y97" s="154"/>
-      <c r="Z97" s="154"/>
-      <c r="AA97" s="154"/>
-      <c r="AB97" s="160">
+    <row r="97" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B97" s="169">
+        <v>800109</v>
+      </c>
+      <c r="C97" s="169">
+        <v>300</v>
+      </c>
+      <c r="D97" s="169">
+        <v>35684</v>
+      </c>
+      <c r="E97" s="169">
+        <v>0</v>
+      </c>
+      <c r="F97" s="169">
+        <v>0</v>
+      </c>
+      <c r="G97" s="169">
+        <v>0</v>
+      </c>
+      <c r="H97" s="169">
+        <v>0</v>
+      </c>
+      <c r="I97" s="169">
+        <v>0</v>
+      </c>
+      <c r="J97" s="169">
+        <v>0</v>
+      </c>
+      <c r="K97" s="169">
+        <v>0</v>
+      </c>
+      <c r="L97" s="169">
+        <v>0</v>
+      </c>
+      <c r="M97" s="169">
+        <v>0</v>
+      </c>
+      <c r="N97" s="169">
+        <v>0</v>
+      </c>
+      <c r="O97" s="169">
+        <v>0</v>
+      </c>
+      <c r="P97" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="169">
+        <v>0</v>
+      </c>
+      <c r="R97" s="169">
+        <v>19014</v>
+      </c>
+      <c r="S97" s="169">
+        <v>0</v>
+      </c>
+      <c r="T97" s="169">
+        <v>35667</v>
+      </c>
+      <c r="U97" s="169">
+        <v>0</v>
+      </c>
+      <c r="V97" s="169">
+        <v>2872</v>
+      </c>
+      <c r="W97" s="169">
+        <v>0</v>
+      </c>
+      <c r="X97" s="169">
+        <v>2656</v>
+      </c>
+      <c r="Y97" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="169">
+        <v>0</v>
+      </c>
+      <c r="AA97" s="169">
+        <v>0</v>
+      </c>
+      <c r="AB97" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>ВОЕННО-МЕДИЦИНСКАЯ АКАДЕМИЯ ИМЕНИ С.М.КИРОВА</v>
       </c>
       <c r="AC97" s="156">
         <f t="shared" si="9"/>
@@ -18692,37 +19361,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A98" s="16"/>
-      <c r="B98" s="154"/>
-      <c r="C98" s="154"/>
-      <c r="D98" s="154"/>
-      <c r="E98" s="154"/>
-      <c r="F98" s="154"/>
-      <c r="G98" s="154"/>
-      <c r="H98" s="154"/>
-      <c r="I98" s="154"/>
-      <c r="J98" s="154"/>
-      <c r="K98" s="154"/>
-      <c r="L98" s="154"/>
-      <c r="M98" s="154"/>
-      <c r="N98" s="154"/>
-      <c r="O98" s="154"/>
-      <c r="P98" s="154"/>
-      <c r="Q98" s="154"/>
-      <c r="R98" s="154"/>
-      <c r="S98" s="154"/>
-      <c r="T98" s="154"/>
-      <c r="U98" s="154"/>
-      <c r="V98" s="154"/>
-      <c r="W98" s="154"/>
-      <c r="X98" s="154"/>
-      <c r="Y98" s="154"/>
-      <c r="Z98" s="154"/>
-      <c r="AA98" s="154"/>
-      <c r="AB98" s="160">
+    <row r="98" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" s="169">
+        <v>731171</v>
+      </c>
+      <c r="C98" s="169">
+        <v>400</v>
+      </c>
+      <c r="D98" s="169">
+        <v>3217</v>
+      </c>
+      <c r="E98" s="169">
+        <v>0</v>
+      </c>
+      <c r="F98" s="169">
+        <v>0</v>
+      </c>
+      <c r="G98" s="169">
+        <v>0</v>
+      </c>
+      <c r="H98" s="169">
+        <v>0</v>
+      </c>
+      <c r="I98" s="169">
+        <v>0</v>
+      </c>
+      <c r="J98" s="169">
+        <v>0</v>
+      </c>
+      <c r="K98" s="169">
+        <v>0</v>
+      </c>
+      <c r="L98" s="169">
+        <v>0</v>
+      </c>
+      <c r="M98" s="169">
+        <v>0</v>
+      </c>
+      <c r="N98" s="169">
+        <v>0</v>
+      </c>
+      <c r="O98" s="169">
+        <v>0</v>
+      </c>
+      <c r="P98" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="169">
+        <v>0</v>
+      </c>
+      <c r="R98" s="169">
+        <v>2916</v>
+      </c>
+      <c r="S98" s="169">
+        <v>0</v>
+      </c>
+      <c r="T98" s="169">
+        <v>3320</v>
+      </c>
+      <c r="U98" s="169">
+        <v>0</v>
+      </c>
+      <c r="V98" s="169">
+        <v>240</v>
+      </c>
+      <c r="W98" s="169">
+        <v>0</v>
+      </c>
+      <c r="X98" s="169">
+        <v>159</v>
+      </c>
+      <c r="Y98" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="169">
+        <v>0</v>
+      </c>
+      <c r="AA98" s="169">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>ФГБУ "НИИ ГРИППА ИМ. А.А. СМОРОДИНЦЕВА" МИНЗДРАВА РОССИИ</v>
       </c>
       <c r="AC98" s="156">
         <f t="shared" si="9"/>
@@ -18772,37 +19495,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A99" s="16"/>
-      <c r="B99" s="154"/>
-      <c r="C99" s="154"/>
-      <c r="D99" s="154"/>
-      <c r="E99" s="154"/>
-      <c r="F99" s="154"/>
-      <c r="G99" s="154"/>
-      <c r="H99" s="154"/>
-      <c r="I99" s="154"/>
-      <c r="J99" s="154"/>
-      <c r="K99" s="154"/>
-      <c r="L99" s="154"/>
-      <c r="M99" s="154"/>
-      <c r="N99" s="154"/>
-      <c r="O99" s="154"/>
-      <c r="P99" s="154"/>
-      <c r="Q99" s="154"/>
-      <c r="R99" s="154"/>
-      <c r="S99" s="154"/>
-      <c r="T99" s="154"/>
-      <c r="U99" s="154"/>
-      <c r="V99" s="154"/>
-      <c r="W99" s="154"/>
-      <c r="X99" s="154"/>
-      <c r="Y99" s="154"/>
-      <c r="Z99" s="154"/>
-      <c r="AA99" s="154"/>
-      <c r="AB99" s="160">
+    <row r="99" spans="1:42" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" s="169">
+        <v>731178</v>
+      </c>
+      <c r="C99" s="169">
+        <v>300</v>
+      </c>
+      <c r="D99" s="169">
+        <v>52813</v>
+      </c>
+      <c r="E99" s="169">
+        <v>0</v>
+      </c>
+      <c r="F99" s="169">
+        <v>0</v>
+      </c>
+      <c r="G99" s="169">
+        <v>0</v>
+      </c>
+      <c r="H99" s="169">
+        <v>0</v>
+      </c>
+      <c r="I99" s="169">
+        <v>0</v>
+      </c>
+      <c r="J99" s="169">
+        <v>0</v>
+      </c>
+      <c r="K99" s="169">
+        <v>0</v>
+      </c>
+      <c r="L99" s="169">
+        <v>0</v>
+      </c>
+      <c r="M99" s="169">
+        <v>0</v>
+      </c>
+      <c r="N99" s="169">
+        <v>0</v>
+      </c>
+      <c r="O99" s="169">
+        <v>0</v>
+      </c>
+      <c r="P99" s="169">
+        <v>59</v>
+      </c>
+      <c r="Q99" s="169">
+        <v>0</v>
+      </c>
+      <c r="R99" s="169">
+        <v>26188</v>
+      </c>
+      <c r="S99" s="169">
+        <v>0</v>
+      </c>
+      <c r="T99" s="169">
+        <v>52481</v>
+      </c>
+      <c r="U99" s="169">
+        <v>0</v>
+      </c>
+      <c r="V99" s="169">
+        <v>728</v>
+      </c>
+      <c r="W99" s="169">
+        <v>0</v>
+      </c>
+      <c r="X99" s="169">
+        <v>720</v>
+      </c>
+      <c r="Y99" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z99" s="169">
+        <v>20</v>
+      </c>
+      <c r="AA99" s="169">
+        <v>1</v>
+      </c>
+      <c r="AB99" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>ФГБУ "РНИИТО ИМ. Р.Р. ВРЕДЕНА" МИНЗДРАВА РОССИИ</v>
       </c>
       <c r="AC99" s="156">
         <f t="shared" si="9"/>
@@ -18853,36 +19630,90 @@
       </c>
     </row>
     <row r="100" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A100" s="16"/>
-      <c r="B100" s="154"/>
-      <c r="C100" s="154"/>
-      <c r="D100" s="154"/>
-      <c r="E100" s="154"/>
-      <c r="F100" s="154"/>
-      <c r="G100" s="154"/>
-      <c r="H100" s="154"/>
-      <c r="I100" s="154"/>
-      <c r="J100" s="154"/>
-      <c r="K100" s="154"/>
-      <c r="L100" s="154"/>
-      <c r="M100" s="154"/>
-      <c r="N100" s="154"/>
-      <c r="O100" s="154"/>
-      <c r="P100" s="154"/>
-      <c r="Q100" s="154"/>
-      <c r="R100" s="154"/>
-      <c r="S100" s="154"/>
-      <c r="T100" s="154"/>
-      <c r="U100" s="154"/>
-      <c r="V100" s="154"/>
-      <c r="W100" s="154"/>
-      <c r="X100" s="154"/>
-      <c r="Y100" s="154"/>
-      <c r="Z100" s="154"/>
-      <c r="AA100" s="154"/>
-      <c r="AB100" s="160">
+      <c r="A100" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="169">
+        <v>78780154</v>
+      </c>
+      <c r="C100" s="169">
+        <v>200</v>
+      </c>
+      <c r="D100" s="169">
+        <v>5877</v>
+      </c>
+      <c r="E100" s="169">
+        <v>0</v>
+      </c>
+      <c r="F100" s="169">
+        <v>0</v>
+      </c>
+      <c r="G100" s="169">
+        <v>0</v>
+      </c>
+      <c r="H100" s="169">
+        <v>0</v>
+      </c>
+      <c r="I100" s="169">
+        <v>0</v>
+      </c>
+      <c r="J100" s="169">
+        <v>0</v>
+      </c>
+      <c r="K100" s="169">
+        <v>0</v>
+      </c>
+      <c r="L100" s="169">
+        <v>0</v>
+      </c>
+      <c r="M100" s="169">
+        <v>0</v>
+      </c>
+      <c r="N100" s="169">
+        <v>0</v>
+      </c>
+      <c r="O100" s="169">
+        <v>0</v>
+      </c>
+      <c r="P100" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="169">
+        <v>0</v>
+      </c>
+      <c r="R100" s="169">
+        <v>5877</v>
+      </c>
+      <c r="S100" s="169">
+        <v>0</v>
+      </c>
+      <c r="T100" s="169">
+        <v>5877</v>
+      </c>
+      <c r="U100" s="169">
+        <v>0</v>
+      </c>
+      <c r="V100" s="169">
+        <v>1582</v>
+      </c>
+      <c r="W100" s="169">
+        <v>0</v>
+      </c>
+      <c r="X100" s="169">
+        <v>1582</v>
+      </c>
+      <c r="Y100" s="169">
+        <v>0</v>
+      </c>
+      <c r="Z100" s="169">
+        <v>0</v>
+      </c>
+      <c r="AA100" s="169">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="160" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>ООО "Медико-санитарная часть №157"</v>
       </c>
       <c r="AC100" s="156">
         <f t="shared" si="9"/>
@@ -18935,11 +19766,11 @@
   </sheetData>
   <autoFilter ref="A3:AB43"/>
   <mergeCells count="24">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
@@ -18954,84 +19785,217 @@
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AE1:AE3"/>
     <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
+  <conditionalFormatting sqref="E1:E93 E101:E1048576">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC1048576">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="75" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD3:AD1000">
-    <cfRule type="cellIs" dxfId="39" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="71" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="72" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="74" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:AA1000">
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+  <conditionalFormatting sqref="Z3:AA93 Z101:AA1000">
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="63" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="64" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3:AF100">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="61" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG3:AG100">
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="57" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3:AH100">
-    <cfRule type="cellIs" dxfId="27" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="54" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="55" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK3:AK100">
+    <cfRule type="cellIs" dxfId="59" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="52" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="53" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL3:AL100">
+    <cfRule type="cellIs" dxfId="56" priority="49" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="50" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM3:AM100">
+    <cfRule type="cellIs" dxfId="54" priority="46" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="48" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN3:AN100">
+    <cfRule type="cellIs" dxfId="51" priority="43" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="44" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="45" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO3:AO100">
+    <cfRule type="cellIs" dxfId="48" priority="41" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="42" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP3:AP100">
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="39" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="40" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB1:AB2">
+    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E94">
+    <cfRule type="cellIs" dxfId="41" priority="34" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z94:AA94">
+    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="32" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95">
+    <cfRule type="cellIs" dxfId="36" priority="29" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="30" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z95:AA95">
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E96">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z96:AA96">
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E97">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z97:AA97">
     <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -19042,60 +20006,60 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL3:AL100">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
-      <formula>1</formula>
+  <conditionalFormatting sqref="E98">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM3:AM100">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="lessThan">
+  <conditionalFormatting sqref="Z98:AA98">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AN3:AN100">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+  <conditionalFormatting sqref="E99">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO3:AO100">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
-      <formula>1</formula>
+  <conditionalFormatting sqref="Z99:AA99">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP3:AP100">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+  <conditionalFormatting sqref="E100">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB1:AB2">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>1</formula>
+  <conditionalFormatting sqref="Z100:AA100">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19111,7 +20075,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B62" sqref="B62:B63"/>
     </sheetView>
   </sheetViews>
@@ -19139,7 +20103,7 @@
       </c>
       <c r="D1" s="110">
         <f>COUNTIF(B2:B1000, "_Должник")</f>
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E1" s="112"/>
       <c r="F1" s="115" t="s">
@@ -19147,7 +20111,7 @@
       </c>
       <c r="G1" s="109">
         <f>COUNTA(Эталон!B2:B1000)-D1</f>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -19397,7 +20361,7 @@
       </c>
       <c r="B26" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A26, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A26)</f>
-        <v>_Должник</v>
+        <v>ООО "Медико-санитарная часть №157"</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -19497,7 +20461,7 @@
       </c>
       <c r="B36" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A36, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A36)</f>
-        <v>_Должник</v>
+        <v>СПб ГБУЗ "Городская Мариинская больница"</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -19527,7 +20491,7 @@
       </c>
       <c r="B39" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A39, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A39)</f>
-        <v>_Должник</v>
+        <v>ВОЕННО-МЕДИЦИНСКАЯ АКАДЕМИЯ ИМЕНИ С.М.КИРОВА</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -19567,7 +20531,7 @@
       </c>
       <c r="B43" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A43, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A43)</f>
-        <v>_Должник</v>
+        <v>ФГБУ "РНИИТО ИМ. Р.Р. ВРЕДЕНА" МИНЗДРАВА РОССИИ</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -19637,7 +20601,7 @@
       </c>
       <c r="B50" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A50, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A50)</f>
-        <v>_Должник</v>
+        <v>ФГБУ "НИИ ГРИППА ИМ. А.А. СМОРОДИНЦЕВА" МИНЗДРАВА РОССИИ</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -19647,7 +20611,7 @@
       </c>
       <c r="B51" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A51, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A51)</f>
-        <v>_Должник</v>
+        <v>СПб ГБУЗ "Городской клинический онкологический диспансер"</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -19677,7 +20641,7 @@
       </c>
       <c r="B54" s="111" t="str">
         <f>IF(ISNA(VLOOKUP(A54, 'Для заполнения'!A:A, 1, FALSE)), "_Должник", A54)</f>
-        <v>_Должник</v>
+        <v>СПб ГБУЗ "Городская больница Святой преподобномученицы Елизаветы"</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -19959,68 +20923,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="218" t="s">
+      <c r="B1" s="215" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="219" t="s">
+      <c r="C1" s="216" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="210" t="s">
+      <c r="D1" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="211" t="s">
+      <c r="E1" s="198" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="211" t="s">
+      <c r="F1" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
-      <c r="N1" s="213"/>
-      <c r="O1" s="213"/>
-      <c r="P1" s="214" t="s">
+      <c r="G1" s="214"/>
+      <c r="H1" s="214"/>
+      <c r="I1" s="214"/>
+      <c r="J1" s="214"/>
+      <c r="K1" s="214"/>
+      <c r="L1" s="214"/>
+      <c r="M1" s="214"/>
+      <c r="N1" s="214"/>
+      <c r="O1" s="214"/>
+      <c r="P1" s="218" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="214" t="s">
+      <c r="Q1" s="218" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="214" t="s">
+      <c r="R1" s="218" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="213"/>
-      <c r="T1" s="215" t="s">
+      <c r="S1" s="214"/>
+      <c r="T1" s="219" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="213"/>
-      <c r="V1" s="216" t="s">
+      <c r="U1" s="214"/>
+      <c r="V1" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="213"/>
-      <c r="X1" s="217" t="s">
+      <c r="W1" s="214"/>
+      <c r="X1" s="221" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="213"/>
-      <c r="Z1" s="212" t="s">
+      <c r="Y1" s="214"/>
+      <c r="Z1" s="217" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="212" t="s">
+      <c r="AA1" s="217" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="220.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="213"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
       <c r="F2" s="130" t="s">
         <v>15</v>
       </c>
@@ -20051,8 +21015,8 @@
       <c r="O2" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="213"/>
-      <c r="Q2" s="213"/>
+      <c r="P2" s="214"/>
+      <c r="Q2" s="214"/>
       <c r="R2" s="131" t="s">
         <v>25</v>
       </c>
@@ -20077,8 +21041,8 @@
       <c r="Y2" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="213"/>
-      <c r="AA2" s="213"/>
+      <c r="Z2" s="214"/>
+      <c r="AA2" s="214"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="134" t="s">
@@ -23001,12 +23965,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="P1:P2"/>
@@ -23015,6 +23973,12 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="F1:O1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E100">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>